<commit_message>
US2 and US3 Done
</commit_message>
<xml_diff>
--- a/DTT-Assessment-Hour-Log_2023.xlsx
+++ b/DTT-Assessment-Hour-Log_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\web_backend_test_catering_api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E762A6A-FD1F-4F4F-80D7-35ADA72C3FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC03ABDF-D2A5-4A29-A837-F028ED4FBA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <r>
       <rPr>
@@ -73,31 +73,54 @@
     <t>Bonus</t>
   </si>
   <si>
-    <t>Example 2</t>
-  </si>
-  <si>
-    <t>Had some issues with…</t>
-  </si>
-  <si>
-    <t>Example 3</t>
-  </si>
-  <si>
-    <t>Implemented bonus feature….</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Total amount of hours</t>
   </si>
   <si>
     <t>User Story 1 and User Story 2(a,b,c)</t>
   </si>
   <si>
-    <t>18/12/2022</t>
-  </si>
-  <si>
     <t>Created databse and implemented create and read API endpoint</t>
+  </si>
+  <si>
+    <t>User Story 2(d,e) and User Story 3</t>
+  </si>
+  <si>
+    <t>19/12/2023</t>
+  </si>
+  <si>
+    <t>18/12/2023</t>
+  </si>
+  <si>
+    <t>Implemented update and delete api endpoints after that implemented search funcionality in read endpoint.</t>
+  </si>
+  <si>
+    <t>Git Version Control</t>
+  </si>
+  <si>
+    <r>
+      <t>Used git version control from the beginning. Link -</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> https://github.com/BadhonRahman01/DTT_Backend_Exam</t>
+    </r>
+  </si>
+  <si>
+    <t>Pagination</t>
+  </si>
+  <si>
+    <t>Implemented pagination on search method in read endpoint.</t>
+  </si>
+  <si>
+    <t>10mins</t>
+  </si>
+  <si>
+    <t>30mins</t>
   </si>
 </sst>
 </file>
@@ -107,7 +130,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
@@ -173,6 +196,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -328,12 +357,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -366,6 +389,12 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -801,7 +830,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.53515625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -814,311 +843,317 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="6">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="8">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="E5" s="9"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="B6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B30" s="14">
+        <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
         <v>3</v>
       </c>
-      <c r="C5" s="9">
-        <v>44562</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="8">
-        <v>5</v>
-      </c>
-      <c r="C6" s="9">
-        <v>44562</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="6"/>
-    </row>
-    <row r="25" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="6"/>
-    </row>
-    <row r="27" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="7"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="6"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="6"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="16">
-        <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>4</v>
-      </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="6"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="6"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="6"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="18"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="20"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>